<commit_message>
Add End of Road boolean to Tile and the Tileset csv
</commit_message>
<xml_diff>
--- a/Tileset.xlsx
+++ b/Tileset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Storm\IdeaProjects\Carcassone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F7332FD-6DE9-489B-8847-BA2CF9B36A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891AD676-6482-4823-A0DE-CF9D7ED39C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{EB2D1F6D-AA63-4B22-B799-6490843261F4}"/>
+    <workbookView xWindow="42645" yWindow="390" windowWidth="28800" windowHeight="13830" xr2:uid="{EB2D1F6D-AA63-4B22-B799-6490843261F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tileset" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="3">
   <si>
     <t>Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Field</t>
@@ -421,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E21B34F-D8ED-4A03-BC22-C0084758B3B8}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="J8:K8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,18 +428,18 @@
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" t="b">
         <v>1</v>
@@ -453,19 +450,22 @@
       <c r="G1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -476,19 +476,22 @@
       <c r="G2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -499,19 +502,22 @@
       <c r="G3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -522,19 +528,22 @@
       <c r="G4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -545,19 +554,22 @@
       <c r="G5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -568,16 +580,19 @@
       <c r="G6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -591,16 +606,19 @@
       <c r="G7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -614,16 +632,19 @@
       <c r="G8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -637,16 +658,19 @@
       <c r="G9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -660,16 +684,19 @@
       <c r="G10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -683,16 +710,19 @@
       <c r="G11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -706,16 +736,19 @@
       <c r="G12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
@@ -729,16 +762,19 @@
       <c r="G13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
         <v>0</v>
@@ -752,13 +788,16 @@
       <c r="G14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
@@ -775,13 +814,16 @@
       <c r="G15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
@@ -796,15 +838,18 @@
         <v>0</v>
       </c>
       <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
@@ -819,15 +864,18 @@
         <v>0</v>
       </c>
       <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
@@ -842,15 +890,18 @@
         <v>0</v>
       </c>
       <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
@@ -865,15 +916,18 @@
         <v>0</v>
       </c>
       <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
@@ -888,15 +942,18 @@
         <v>0</v>
       </c>
       <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
@@ -911,15 +968,18 @@
         <v>0</v>
       </c>
       <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
@@ -934,15 +994,18 @@
         <v>0</v>
       </c>
       <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
@@ -957,12 +1020,15 @@
         <v>0</v>
       </c>
       <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -981,11 +1047,14 @@
       </c>
       <c r="G24" t="b">
         <v>0</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
@@ -1004,11 +1073,14 @@
       </c>
       <c r="G25" t="b">
         <v>0</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -1027,11 +1099,14 @@
       </c>
       <c r="G26" t="b">
         <v>0</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
@@ -1050,6 +1125,9 @@
       </c>
       <c r="G27" t="b">
         <v>0</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1074,22 +1152,22 @@
       <c r="G28" t="b">
         <v>0</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -1098,21 +1176,24 @@
         <v>0</v>
       </c>
       <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -1121,21 +1202,24 @@
         <v>0</v>
       </c>
       <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -1144,21 +1228,24 @@
         <v>0</v>
       </c>
       <c r="G31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -1169,19 +1256,22 @@
       <c r="G32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -1192,16 +1282,19 @@
       <c r="G33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
         <v>0</v>
@@ -1215,16 +1308,19 @@
       <c r="G34" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" t="s">
         <v>0</v>
@@ -1238,16 +1334,19 @@
       <c r="G35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
         <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
         <v>0</v>
@@ -1261,16 +1360,19 @@
       <c r="G36" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" t="s">
         <v>0</v>
@@ -1284,13 +1386,16 @@
       <c r="G37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" t="s">
         <v>0</v>
@@ -1307,13 +1412,16 @@
       <c r="G38" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" t="s">
         <v>0</v>
@@ -1330,13 +1438,16 @@
       <c r="G39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
@@ -1353,10 +1464,13 @@
       <c r="G40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B41" t="s">
         <v>0</v>
@@ -1365,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
@@ -1376,10 +1490,13 @@
       <c r="G41" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B42" t="s">
         <v>0</v>
@@ -1388,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -1399,10 +1516,13 @@
       <c r="G42" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B43" t="s">
         <v>0</v>
@@ -1411,7 +1531,7 @@
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -1422,10 +1542,13 @@
       <c r="G43" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B44" t="s">
         <v>0</v>
@@ -1445,10 +1568,13 @@
       <c r="G44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B45" t="s">
         <v>0</v>
@@ -1468,10 +1594,13 @@
       <c r="G45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B46" t="s">
         <v>0</v>
@@ -1491,19 +1620,22 @@
       <c r="G46" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
@@ -1514,19 +1646,22 @@
       <c r="G47" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -1537,19 +1672,22 @@
       <c r="G48" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -1560,19 +1698,22 @@
       <c r="G49" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -1583,19 +1724,22 @@
       <c r="G50" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -1606,19 +1750,22 @@
       <c r="G51" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
@@ -1629,19 +1776,22 @@
       <c r="G52" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
@@ -1652,19 +1802,22 @@
       <c r="G53" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
@@ -1675,19 +1828,22 @@
       <c r="G54" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
@@ -1698,13 +1854,16 @@
       <c r="G55" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
         <v>0</v>
@@ -1721,13 +1880,16 @@
       <c r="G56" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C57" t="s">
         <v>0</v>
@@ -1744,13 +1906,16 @@
       <c r="G57" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C58" t="s">
         <v>0</v>
@@ -1767,19 +1932,22 @@
       <c r="G58" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
@@ -1790,19 +1958,22 @@
       <c r="G59" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E60" t="b">
         <v>0</v>
@@ -1813,19 +1984,22 @@
       <c r="G60" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
@@ -1836,19 +2010,22 @@
       <c r="G61" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E62" t="b">
         <v>0</v>
@@ -1859,13 +2036,16 @@
       <c r="G62" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63" t="s">
         <v>0</v>
@@ -1882,13 +2062,16 @@
       <c r="G63" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C64" t="s">
         <v>0</v>
@@ -1905,19 +2088,22 @@
       <c r="G64" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E65" t="b">
         <v>0</v>
@@ -1928,19 +2114,22 @@
       <c r="G65" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B66" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E66" t="b">
         <v>0</v>
@@ -1951,19 +2140,22 @@
       <c r="G66" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B67" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C67" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E67" t="b">
         <v>0</v>
@@ -1974,19 +2166,22 @@
       <c r="G67" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B68" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C68" t="s">
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E68" t="b">
         <v>0</v>
@@ -1997,19 +2192,22 @@
       <c r="G68" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B69" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
@@ -2020,19 +2218,22 @@
       <c r="G69" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B70" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C70" t="s">
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E70" t="b">
         <v>0</v>
@@ -2043,19 +2244,22 @@
       <c r="G70" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B71" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71" t="s">
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E71" t="b">
         <v>0</v>
@@ -2066,19 +2270,22 @@
       <c r="G71" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B72" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C72" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E72" t="b">
         <v>0</v>
@@ -2089,9 +2296,12 @@
       <c r="G72" t="b">
         <v>1</v>
       </c>
+      <c r="H72" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:E54 F29:G54 A55:G65 E68:E267 E66:G67 A66:D76 F68:G72">
+  <conditionalFormatting sqref="A1:E54 F29:G54 A55:G65 E68:E267 E66:G67 A66:D76 F68:G72 H1:H72">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"City"</formula>
     </cfRule>
@@ -2102,7 +2312,7 @@
       <formula>"Field"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E54 F29:G54 E68:E267 E55:G67 F68:G72">
+  <conditionalFormatting sqref="E1:E54 F29:G54 E68:E267 E55:G67 F68:G72 H1:H72">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2112,7 +2322,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1">
+  <conditionalFormatting sqref="H1:H72 E1">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>